<commit_message>
opdateret iteration og faseplan
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -136,9 +136,6 @@
     <t>Påbegynde Domænemodel</t>
   </si>
   <si>
-    <t>Ikke funktionelle krav</t>
-  </si>
-  <si>
     <t>Mockups</t>
   </si>
   <si>
@@ -146,6 +143,15 @@
   </si>
   <si>
     <t>Aflevering af projekt</t>
+  </si>
+  <si>
+    <t>Review af artefakter med gruppe grp 2</t>
+  </si>
+  <si>
+    <t>Lav UC1</t>
+  </si>
+  <si>
+    <t>Lav UC2</t>
   </si>
 </sst>
 </file>
@@ -555,7 +561,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -569,7 +575,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -828,6 +834,9 @@
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
+      <c r="K6" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -838,7 +847,7 @@
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
       <c r="AC6" s="20" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -848,7 +857,9 @@
       <c r="D7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="10"/>
+      <c r="E7" s="10" t="s">
+        <v>29</v>
+      </c>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
@@ -875,7 +886,9 @@
       <c r="D8" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="20"/>
+      <c r="E8" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="K8" s="14"/>
@@ -897,6 +910,9 @@
       <c r="D9" t="s">
         <v>37</v>
       </c>
+      <c r="E9" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="9"/>
@@ -915,7 +931,10 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>38</v>
+        <v>42</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -931,7 +950,10 @@
     </row>
     <row r="11" spans="1:29">
       <c r="D11" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -944,7 +966,7 @@
     </row>
     <row r="12" spans="1:29">
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -959,6 +981,12 @@
       <c r="AC12" s="7"/>
     </row>
     <row r="13" spans="1:29">
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>29</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="9"/>
@@ -988,9 +1016,6 @@
       <c r="AC14" s="8"/>
     </row>
     <row r="15" spans="1:29">
-      <c r="D15" s="7" t="s">
-        <v>1</v>
-      </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1000,17 +1025,13 @@
       <c r="P15" s="2"/>
     </row>
     <row r="16" spans="1:29">
-      <c r="D16" s="8" t="s">
-        <v>2</v>
-      </c>
+      <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
     <row r="17" spans="4:19">
-      <c r="D17" s="8" t="s">
-        <v>31</v>
-      </c>
+      <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
@@ -1018,9 +1039,7 @@
       <c r="N17" s="7"/>
     </row>
     <row r="18" spans="4:19">
-      <c r="D18" s="8" t="s">
-        <v>30</v>
-      </c>
+      <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
@@ -1030,9 +1049,7 @@
       <c r="N18" s="8"/>
     </row>
     <row r="19" spans="4:19">
-      <c r="D19" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
@@ -1043,9 +1060,7 @@
       <c r="N19" s="8"/>
     </row>
     <row r="20" spans="4:19">
-      <c r="D20" s="8" t="s">
-        <v>11</v>
-      </c>
+      <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
@@ -1056,6 +1071,7 @@
       <c r="N20" s="8"/>
     </row>
     <row r="21" spans="4:19">
+      <c r="D21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="K21"/>

</xml_diff>

<commit_message>
iteration og faseplan opdateret
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -152,6 +152,30 @@
   </si>
   <si>
     <t>Lav UC2</t>
+  </si>
+  <si>
+    <t>System sekvens diagrammer</t>
+  </si>
+  <si>
+    <t>2 timer</t>
+  </si>
+  <si>
+    <t>Review af gruppe 2s artefakter</t>
+  </si>
+  <si>
+    <t>Operations kontraker</t>
+  </si>
+  <si>
+    <t>rapport skrivning</t>
+  </si>
+  <si>
+    <t>database model og normalformer</t>
+  </si>
+  <si>
+    <t>3 timer</t>
+  </si>
+  <si>
+    <t>Klassediagram med fokus på 3lags deling</t>
   </si>
 </sst>
 </file>
@@ -561,7 +585,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,10 +596,10 @@
   <dimension ref="A1:AC35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -830,8 +854,12 @@
       <c r="E6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
+      <c r="F6" s="20" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="K6" s="10" t="s">
@@ -860,8 +888,12 @@
       <c r="E7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="F7" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
       <c r="K7" s="14"/>
@@ -889,8 +921,12 @@
       <c r="E8" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20"/>
+      <c r="F8" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="K8" s="14"/>
       <c r="U8" s="10"/>
       <c r="W8" s="7"/>
@@ -912,6 +948,12 @@
       </c>
       <c r="E9" s="20" t="s">
         <v>34</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -935,6 +977,12 @@
       </c>
       <c r="E10" s="20" t="s">
         <v>29</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>50</v>
       </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -954,6 +1002,12 @@
       </c>
       <c r="E11" s="20" t="s">
         <v>34</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>29</v>
       </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>

</xml_diff>

<commit_message>
projektplan opdateret med iterationsplan for E1
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -2,13 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
     <sheet name="Milepæle" sheetId="4" r:id="rId2"/>
+    <sheet name="Ark1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -176,6 +177,39 @@
   </si>
   <si>
     <t>Klassediagram med fokus på 3lags deling</t>
+  </si>
+  <si>
+    <t>forberedelse til møde med hans</t>
+  </si>
+  <si>
+    <t>møde med hans</t>
+  </si>
+  <si>
+    <t>20 min</t>
+  </si>
+  <si>
+    <t>implementation af feedback fra hans</t>
+  </si>
+  <si>
+    <t>Plan</t>
+  </si>
+  <si>
+    <t>Lave ikke funktionelle krav (FURPS)</t>
+  </si>
+  <si>
+    <t>Identificer alle use cases.</t>
+  </si>
+  <si>
+    <t>Formel beskriv UC3 – opret lånetilbud</t>
+  </si>
+  <si>
+    <t>Sekvens diagram for UC1 og UC2</t>
+  </si>
+  <si>
+    <t>Opdatere klasse diagram</t>
+  </si>
+  <si>
+    <t>Implementere UC1 og UC2.</t>
   </si>
 </sst>
 </file>
@@ -585,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -593,13 +627,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -860,8 +895,12 @@
       <c r="G6" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="H6" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="K6" s="10" t="s">
         <v>41</v>
       </c>
@@ -894,8 +933,12 @@
       <c r="G7" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="H7" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="K7" s="14"/>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
@@ -926,6 +969,12 @@
       </c>
       <c r="G8" s="20" t="s">
         <v>29</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>54</v>
       </c>
       <c r="K8" s="14"/>
       <c r="U8" s="10"/>
@@ -1227,20 +1276,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F7"/>
+  <sheetPr codeName="Ark2"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12"/>
+      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="26" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1283,29 +1334,62 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="C6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B15" s="8" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="B4" s="8" t="s">
+    <row r="16" spans="1:6">
+      <c r="B16" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="B5" s="8" t="s">
+    <row r="17" spans="2:2">
+      <c r="B17" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="B6" s="8" t="s">
+    <row r="18" spans="2:2">
+      <c r="B18" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="B7" s="8" t="s">
+    <row r="19" spans="2:2">
+      <c r="B19" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1313,4 +1397,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr codeName="Ark3"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FURPS tilføjet, projekt plan opdateret
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
     <sheet name="Milepæle" sheetId="4" r:id="rId2"/>
-    <sheet name="Ark1" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -210,6 +209,27 @@
   </si>
   <si>
     <t>Implementere UC1 og UC2.</t>
+  </si>
+  <si>
+    <t>Lavet iterations plan for E1</t>
+  </si>
+  <si>
+    <t>30 min</t>
+  </si>
+  <si>
+    <t>Identificeret de sidste use cases.</t>
+  </si>
+  <si>
+    <t>1,5 timer</t>
+  </si>
+  <si>
+    <t>FURPS og ikke funktionelle krav</t>
+  </si>
+  <si>
+    <t>Oprettet Database</t>
+  </si>
+  <si>
+    <t>Lavet java klasser</t>
   </si>
 </sst>
 </file>
@@ -619,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -628,45 +648,46 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AC35"/>
+  <dimension ref="A1:AD44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="F4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="41.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" customWidth="1"/>
-    <col min="8" max="8" width="32.85546875" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.28515625" customWidth="1"/>
-    <col min="15" max="15" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="35" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="34.28515625" customWidth="1"/>
-    <col min="20" max="20" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="35.28515625" style="10" customWidth="1"/>
-    <col min="25" max="25" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="29" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="35" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="34.28515625" customWidth="1"/>
+    <col min="21" max="21" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.28515625" style="10" customWidth="1"/>
+    <col min="26" max="26" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="30" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:30" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -678,20 +699,21 @@
         <v>5</v>
       </c>
       <c r="K1" s="16"/>
-      <c r="M1" s="16"/>
+      <c r="L1" s="16"/>
       <c r="N1" s="16"/>
-      <c r="O1" s="15"/>
-      <c r="T1" s="15" t="s">
+      <c r="O1" s="16"/>
+      <c r="P1" s="15"/>
+      <c r="U1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="V1" s="16"/>
       <c r="W1" s="16"/>
       <c r="X1" s="16"/>
-      <c r="Y1" s="15" t="s">
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="18" customFormat="1">
+    <row r="2" spans="1:30" s="18" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -703,19 +725,20 @@
         <v>8</v>
       </c>
       <c r="K2" s="19"/>
-      <c r="O2" s="17" t="s">
+      <c r="L2" s="19"/>
+      <c r="P2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="U2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="W2" s="19"/>
       <c r="X2" s="19"/>
-      <c r="Y2" s="17" t="s">
+      <c r="Y2" s="19"/>
+      <c r="Z2" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="5" customFormat="1">
+    <row r="3" spans="1:30" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -732,71 +755,72 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3">
-        <v>43222</v>
+        <v>43223</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="4">
-        <v>43227</v>
-      </c>
-      <c r="K3" s="3">
+        <v>43223</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3">
         <v>43228</v>
       </c>
-      <c r="L3" s="3">
+      <c r="M3" s="3">
         <v>43229</v>
       </c>
-      <c r="M3" s="3">
+      <c r="N3" s="3">
         <v>43230</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>43231</v>
       </c>
-      <c r="O3" s="4">
+      <c r="P3" s="4">
         <v>43234</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>43235</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>43236</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>43237</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>43238</v>
       </c>
-      <c r="T3" s="4">
+      <c r="U3" s="4">
         <v>43241</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>43242</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>43243</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>43244</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>43245</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>43248</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>43249</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>43250</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>43251</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:30">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -812,13 +836,8 @@
       <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" t="s">
+      <c r="K4" s="1"/>
+      <c r="L4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="M4" t="s">
@@ -827,10 +846,10 @@
       <c r="N4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P4" t="s">
+      <c r="O4" t="s">
+        <v>3</v>
+      </c>
+      <c r="P4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Q4" t="s">
@@ -842,25 +861,25 @@
       <c r="S4" t="s">
         <v>3</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="T4" t="s">
+        <v>3</v>
+      </c>
+      <c r="U4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="V4" t="s">
         <v>3</v>
       </c>
-      <c r="W4" s="10" t="s">
+      <c r="W4" t="s">
         <v>3</v>
       </c>
       <c r="X4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="Y4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="Z4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AA4" t="s">
@@ -872,11 +891,14 @@
       <c r="AC4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:29">
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:29">
+      <c r="AD4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30">
+      <c r="M5" s="10"/>
+    </row>
+    <row r="6" spans="1:30">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -901,23 +923,23 @@
       <c r="I6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="L6" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="W6"/>
+      <c r="O6" s="10"/>
+      <c r="V6" s="10"/>
       <c r="X6"/>
-      <c r="Z6" s="20"/>
+      <c r="Y6"/>
       <c r="AA6" s="20"/>
       <c r="AB6" s="20"/>
-      <c r="AC6" s="20" t="s">
+      <c r="AC6" s="20"/>
+      <c r="AD6" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:29">
+    <row r="7" spans="1:30">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -939,19 +961,24 @@
       <c r="I7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="10"/>
+      <c r="J7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="W7"/>
+      <c r="O7" s="10"/>
+      <c r="V7" s="10"/>
       <c r="X7"/>
-      <c r="Z7" s="20"/>
+      <c r="Y7"/>
       <c r="AA7" s="20"/>
       <c r="AB7" s="20"/>
       <c r="AC7" s="20"/>
-    </row>
-    <row r="8" spans="1:29">
+      <c r="AD7" s="20"/>
+    </row>
+    <row r="8" spans="1:30">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -976,16 +1003,21 @@
       <c r="I8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="K8" s="14"/>
-      <c r="U8" s="10"/>
-      <c r="W8" s="7"/>
+      <c r="J8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="10"/>
       <c r="X8" s="7"/>
-      <c r="Z8" s="20"/>
+      <c r="Y8" s="7"/>
       <c r="AA8" s="20"/>
       <c r="AB8" s="20"/>
       <c r="AC8" s="20"/>
-    </row>
-    <row r="9" spans="1:29">
+      <c r="AD8" s="20"/>
+    </row>
+    <row r="9" spans="1:30">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1004,17 +1036,26 @@
       <c r="G9" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="9"/>
-      <c r="L9" s="10"/>
-      <c r="P9" s="2"/>
-      <c r="U9" s="10"/>
-      <c r="W9" s="8"/>
+      <c r="H9" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="M9" s="10"/>
+      <c r="Q9" s="2"/>
+      <c r="V9" s="10"/>
       <c r="X9" s="8"/>
-      <c r="Y9" s="9"/>
-    </row>
-    <row r="10" spans="1:29">
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="9"/>
+    </row>
+    <row r="10" spans="1:30">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1033,19 +1074,22 @@
       <c r="G10" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="9"/>
-      <c r="P10" s="2"/>
-      <c r="U10" s="10"/>
-      <c r="W10" s="8"/>
+      <c r="J10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="2"/>
+      <c r="V10" s="10"/>
       <c r="X10" s="8"/>
-      <c r="Z10" s="20"/>
+      <c r="Y10" s="8"/>
       <c r="AA10" s="20"/>
       <c r="AB10" s="20"/>
       <c r="AC10" s="20"/>
-    </row>
-    <row r="11" spans="1:29">
+      <c r="AD10" s="20"/>
+    </row>
+    <row r="11" spans="1:30">
       <c r="D11" t="s">
         <v>43</v>
       </c>
@@ -1058,215 +1102,256 @@
       <c r="G11" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="9"/>
-      <c r="P11" s="2"/>
-      <c r="T11" s="9"/>
-      <c r="U11" s="10"/>
-      <c r="W11" s="8"/>
+      <c r="J11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K11" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q11" s="2"/>
+      <c r="U11" s="9"/>
+      <c r="V11" s="10"/>
       <c r="X11" s="8"/>
-    </row>
-    <row r="12" spans="1:29">
+      <c r="Y11" s="8"/>
+    </row>
+    <row r="12" spans="1:30">
       <c r="D12" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="9"/>
-      <c r="P12" s="2"/>
-      <c r="U12" s="10"/>
-      <c r="W12" s="8"/>
+      <c r="J12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12" s="2"/>
+      <c r="V12" s="10"/>
       <c r="X12" s="8"/>
-      <c r="Z12" s="7"/>
+      <c r="Y12" s="8"/>
       <c r="AA12" s="7"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
-    </row>
-    <row r="13" spans="1:29">
+      <c r="AD12" s="7"/>
+    </row>
+    <row r="13" spans="1:30">
       <c r="D13" t="s">
         <v>39</v>
       </c>
       <c r="E13" t="s">
         <v>29</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="9"/>
-      <c r="L13" s="10"/>
-      <c r="P13" s="2"/>
-      <c r="U13" s="10"/>
-      <c r="W13" s="8"/>
+      <c r="M13" s="10"/>
+      <c r="Q13" s="2"/>
+      <c r="V13" s="10"/>
       <c r="X13" s="8"/>
-      <c r="Z13" s="8"/>
+      <c r="Y13" s="8"/>
       <c r="AA13" s="8"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
-    </row>
-    <row r="14" spans="1:29">
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="9"/>
-      <c r="K14"/>
-      <c r="L14" s="10"/>
-      <c r="P14" s="2"/>
-      <c r="U14" s="10"/>
-      <c r="W14" s="8"/>
+      <c r="AD13" s="8"/>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="L14"/>
+      <c r="M14" s="10"/>
+      <c r="Q14" s="2"/>
+      <c r="V14" s="10"/>
       <c r="X14" s="8"/>
-      <c r="Z14" s="8"/>
+      <c r="Y14" s="8"/>
       <c r="AA14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
-    </row>
-    <row r="15" spans="1:29">
+      <c r="AD14" s="8"/>
+    </row>
+    <row r="15" spans="1:30">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
       <c r="J15" s="9"/>
-      <c r="P15" s="2"/>
-    </row>
-    <row r="16" spans="1:29">
+      <c r="Q15" s="2"/>
+    </row>
+    <row r="16" spans="1:30">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
     </row>
-    <row r="17" spans="4:19">
+    <row r="17" spans="4:20">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-      <c r="M17" s="7"/>
       <c r="N17" s="7"/>
-    </row>
-    <row r="18" spans="4:19">
+      <c r="O17" s="7"/>
+    </row>
+    <row r="18" spans="4:20">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
       <c r="I18" s="7"/>
-      <c r="M18" s="8"/>
       <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="4:19">
+      <c r="O18" s="8"/>
+    </row>
+    <row r="19" spans="4:20">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="K19"/>
-      <c r="M19" s="8"/>
+      <c r="L19"/>
       <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="4:19">
+      <c r="O19" s="8"/>
+    </row>
+    <row r="20" spans="4:20">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="K20"/>
-      <c r="M20" s="8"/>
+      <c r="L20"/>
       <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="4:19">
+      <c r="O20" s="8"/>
+    </row>
+    <row r="21" spans="4:20">
       <c r="D21" s="8"/>
-      <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="K21"/>
-      <c r="M21" s="8"/>
+      <c r="L21"/>
       <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="4:19">
+      <c r="O21" s="8"/>
+    </row>
+    <row r="22" spans="4:20">
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="K22"/>
-      <c r="M22" s="8"/>
+      <c r="L22"/>
       <c r="N22" s="8"/>
-      <c r="Q22" s="7"/>
+      <c r="O22" s="8"/>
       <c r="R22" s="7"/>
       <c r="S22" s="7"/>
-    </row>
-    <row r="23" spans="4:19">
+      <c r="T22" s="7"/>
+    </row>
+    <row r="23" spans="4:20">
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="K23"/>
-      <c r="M23" s="8"/>
+      <c r="L23"/>
       <c r="N23" s="8"/>
-      <c r="Q23" s="8"/>
+      <c r="O23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
-    </row>
-    <row r="24" spans="4:19">
+      <c r="T23" s="8"/>
+    </row>
+    <row r="24" spans="4:20">
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="K24"/>
-      <c r="M24" s="8"/>
+      <c r="L24"/>
       <c r="N24" s="8"/>
-      <c r="Q24" s="8"/>
+      <c r="O24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
-    </row>
-    <row r="25" spans="4:19">
+      <c r="T24" s="8"/>
+    </row>
+    <row r="25" spans="4:20">
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
-    </row>
-    <row r="26" spans="4:19">
-      <c r="Q26" s="8"/>
+      <c r="T25" s="8"/>
+    </row>
+    <row r="26" spans="4:20">
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
-    </row>
-    <row r="27" spans="4:19">
-      <c r="Q27" s="8"/>
+      <c r="T26" s="8"/>
+    </row>
+    <row r="27" spans="4:20">
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
-    </row>
-    <row r="28" spans="4:19">
-      <c r="Q28" s="8"/>
+      <c r="T27" s="8"/>
+    </row>
+    <row r="28" spans="4:20">
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
-    </row>
-    <row r="29" spans="4:19">
-      <c r="Q29" s="8"/>
+      <c r="T28" s="8"/>
+    </row>
+    <row r="29" spans="4:20">
+      <c r="I29" s="2"/>
+      <c r="K29" s="14"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
-    </row>
-    <row r="30" spans="4:19">
-      <c r="Q30" s="8"/>
+      <c r="T29" s="8"/>
+    </row>
+    <row r="30" spans="4:20">
+      <c r="I30" s="2"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
-    </row>
-    <row r="31" spans="4:19">
-      <c r="Q31" s="8"/>
+      <c r="T30" s="8"/>
+    </row>
+    <row r="31" spans="4:20">
+      <c r="I31" s="2"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="14"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
-    </row>
-    <row r="32" spans="4:19">
-      <c r="Q32" s="8"/>
+      <c r="T31" s="8"/>
+    </row>
+    <row r="32" spans="4:20">
+      <c r="H32" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
-    </row>
-    <row r="33" spans="17:19">
-      <c r="Q33" s="8"/>
+      <c r="T32" s="8"/>
+    </row>
+    <row r="33" spans="8:20">
+      <c r="H33" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="14"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
-    </row>
-    <row r="34" spans="17:19">
-      <c r="Q34" s="8"/>
+      <c r="T33" s="8"/>
+    </row>
+    <row r="34" spans="8:20">
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="14"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
-    </row>
-    <row r="35" spans="17:19">
-      <c r="Q35" s="8"/>
+      <c r="T34" s="8"/>
+    </row>
+    <row r="35" spans="8:20">
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="14"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
+      <c r="T35" s="8"/>
+    </row>
+    <row r="36" spans="8:20">
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="8:20">
+      <c r="H37" s="2"/>
+    </row>
+    <row r="38" spans="8:20">
+      <c r="H38" s="2"/>
+    </row>
+    <row r="41" spans="8:20">
+      <c r="H41" s="7"/>
+    </row>
+    <row r="42" spans="8:20">
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="8:20">
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="8:20">
+      <c r="H44" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -1279,11 +1364,11 @@
   <sheetPr codeName="Ark2"/>
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C12" sqref="C12"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1397,19 +1482,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Ark3"/>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
opdateret IP og FP, lavet log for dag 4
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t>Lavet java klasser</t>
+  </si>
+  <si>
+    <t>skrevet rapport 2</t>
+  </si>
+  <si>
+    <t>revidering af usecasemodel</t>
+  </si>
+  <si>
+    <t>lavet dataordbog</t>
   </si>
 </sst>
 </file>
@@ -639,7 +648,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -651,10 +660,10 @@
   <dimension ref="A1:AD44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J19" sqref="J19"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1140,6 +1149,12 @@
       <c r="E13" t="s">
         <v>29</v>
       </c>
+      <c r="J13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K13" s="20" t="s">
+        <v>45</v>
+      </c>
       <c r="M13" s="10"/>
       <c r="Q13" s="2"/>
       <c r="V13" s="10"/>
@@ -1151,6 +1166,12 @@
       <c r="AD13" s="8"/>
     </row>
     <row r="14" spans="1:30">
+      <c r="J14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="L14"/>
       <c r="M14" s="10"/>
       <c r="Q14" s="2"/>
@@ -1166,7 +1187,13 @@
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-      <c r="J15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>34</v>
+      </c>
       <c r="Q15" s="2"/>
     </row>
     <row r="16" spans="1:30">
@@ -1174,12 +1201,14 @@
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="4:20">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
+      <c r="I17" s="1"/>
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
     </row>
@@ -1188,7 +1217,7 @@
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
-      <c r="I18" s="7"/>
+      <c r="I18" s="1"/>
       <c r="N18" s="8"/>
       <c r="O18" s="8"/>
     </row>
@@ -1197,7 +1226,7 @@
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
-      <c r="I19" s="8"/>
+      <c r="I19" s="1"/>
       <c r="L19"/>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
@@ -1207,21 +1236,21 @@
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
-      <c r="I20" s="8"/>
+      <c r="I20" s="1"/>
       <c r="L20"/>
       <c r="N20" s="8"/>
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="4:20">
       <c r="D21" s="8"/>
-      <c r="I21" s="8"/>
+      <c r="I21" s="1"/>
       <c r="L21"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
     </row>
     <row r="22" spans="4:20">
       <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
+      <c r="I22" s="1"/>
       <c r="L22"/>
       <c r="N22" s="8"/>
       <c r="O22" s="8"/>
@@ -1231,7 +1260,7 @@
     </row>
     <row r="23" spans="4:20">
       <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
+      <c r="I23" s="1"/>
       <c r="L23"/>
       <c r="N23" s="8"/>
       <c r="O23" s="8"/>
@@ -1241,7 +1270,7 @@
     </row>
     <row r="24" spans="4:20">
       <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
+      <c r="I24" s="1"/>
       <c r="L24"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -1251,28 +1280,31 @@
     </row>
     <row r="25" spans="4:20">
       <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
+      <c r="I25" s="1"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
     </row>
     <row r="26" spans="4:20">
+      <c r="I26" s="1"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
     </row>
     <row r="27" spans="4:20">
+      <c r="I27" s="1"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
     </row>
     <row r="28" spans="4:20">
+      <c r="I28" s="1"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
     </row>
     <row r="29" spans="4:20">
-      <c r="I29" s="2"/>
+      <c r="I29" s="1"/>
       <c r="K29" s="14"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
@@ -1280,7 +1312,6 @@
     </row>
     <row r="30" spans="4:20">
       <c r="I30" s="2"/>
-      <c r="J30" s="9"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="R30" s="8"/>
@@ -1289,7 +1320,6 @@
     </row>
     <row r="31" spans="4:20">
       <c r="I31" s="2"/>
-      <c r="J31" s="9"/>
       <c r="K31" s="14"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -1298,7 +1328,6 @@
     <row r="32" spans="4:20">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
-      <c r="J32" s="9"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="R32" s="8"/>
@@ -1308,7 +1337,6 @@
     <row r="33" spans="8:20">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
-      <c r="J33" s="9"/>
       <c r="K33" s="14"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -1317,7 +1345,6 @@
     <row r="34" spans="8:20">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
-      <c r="J34" s="9"/>
       <c r="K34" s="14"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
@@ -1326,7 +1353,6 @@
     <row r="35" spans="8:20">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
-      <c r="J35" s="9"/>
       <c r="K35" s="14"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>

</xml_diff>

<commit_message>
opdateret rapport, visions dokument og IP/FP
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -145,9 +145,6 @@
     <t>Aflevering af projekt</t>
   </si>
   <si>
-    <t>Review af artefakter med gruppe grp 2</t>
-  </si>
-  <si>
     <t>Lav UC1</t>
   </si>
   <si>
@@ -239,6 +236,12 @@
   </si>
   <si>
     <t>lavet dataordbog</t>
+  </si>
+  <si>
+    <t>Review af eksisterende afsnit i rapport</t>
+  </si>
+  <si>
+    <t>skrive rapport om 3 lags model</t>
   </si>
 </sst>
 </file>
@@ -648,7 +651,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -660,10 +663,10 @@
   <dimension ref="A1:AD44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -679,7 +682,7 @@
     <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="34.28515625" customWidth="1"/>
@@ -772,7 +775,7 @@
       </c>
       <c r="K3" s="3"/>
       <c r="L3" s="3">
-        <v>43228</v>
+        <v>43224</v>
       </c>
       <c r="M3" s="3">
         <v>43229</v>
@@ -921,19 +924,19 @@
         <v>34</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>45</v>
-      </c>
       <c r="H6" s="20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>41</v>
+        <v>53</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -959,22 +962,25 @@
         <v>29</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="20" t="s">
         <v>34</v>
       </c>
       <c r="H7" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>29</v>
+      </c>
+      <c r="L7" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
@@ -1001,22 +1007,22 @@
         <v>34</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" s="20" t="s">
         <v>29</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J8" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>53</v>
-      </c>
-      <c r="K8" s="20" t="s">
-        <v>54</v>
       </c>
       <c r="V8" s="10"/>
       <c r="X8" s="7"/>
@@ -1040,22 +1046,22 @@
         <v>34</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H9" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="I9" s="20" t="s">
+      <c r="J9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="20" t="s">
         <v>65</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>66</v>
       </c>
       <c r="M9" s="10"/>
       <c r="Q9" s="2"/>
@@ -1072,22 +1078,22 @@
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>29</v>
       </c>
       <c r="F10" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="G10" s="20" t="s">
-        <v>50</v>
-      </c>
       <c r="J10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="V10" s="10"/>
@@ -1100,22 +1106,22 @@
     </row>
     <row r="11" spans="1:30">
       <c r="D11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="20" t="s">
         <v>29</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="U11" s="9"/>
@@ -1128,7 +1134,7 @@
         <v>38</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K12" s="20" t="s">
         <v>34</v>
@@ -1150,10 +1156,10 @@
         <v>29</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M13" s="10"/>
       <c r="Q13" s="2"/>
@@ -1167,7 +1173,7 @@
     </row>
     <row r="14" spans="1:30">
       <c r="J14" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="K14" s="20" t="s">
         <v>34</v>
@@ -1189,7 +1195,7 @@
       <c r="G15" s="7"/>
       <c r="I15" s="9"/>
       <c r="J15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K15" s="20" t="s">
         <v>34</v>
@@ -1445,35 +1451,35 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="C5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="C6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="C7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="C8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:6">

</xml_diff>

<commit_message>
lavet formel UC3 opdateret IP/FP
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="77">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -242,6 +242,15 @@
   </si>
   <si>
     <t>skrive rapport om 3 lags model</t>
+  </si>
+  <si>
+    <t>1,25 timer</t>
+  </si>
+  <si>
+    <t>formel beskriv UC3</t>
+  </si>
+  <si>
+    <t>skrive rapport om datamodel og normalisering</t>
   </si>
 </sst>
 </file>
@@ -651,7 +660,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -660,13 +669,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AD44"/>
+  <dimension ref="A1:AE44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -682,24 +691,25 @@
     <col min="9" max="9" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="30.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.28515625" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="34.28515625" customWidth="1"/>
-    <col min="21" max="21" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.28515625" style="10" customWidth="1"/>
-    <col min="26" max="26" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="30" width="28.7109375" customWidth="1"/>
+    <col min="12" max="12" width="43" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="10" customWidth="1"/>
+    <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="34.28515625" customWidth="1"/>
+    <col min="22" max="22" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.28515625" style="10" customWidth="1"/>
+    <col min="27" max="27" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="31" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:31" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -712,20 +722,21 @@
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
-      <c r="N1" s="16"/>
+      <c r="M1" s="16"/>
       <c r="O1" s="16"/>
-      <c r="P1" s="15"/>
-      <c r="U1" s="15" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="15"/>
+      <c r="V1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="16"/>
       <c r="X1" s="16"/>
       <c r="Y1" s="16"/>
-      <c r="Z1" s="15" t="s">
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="18" customFormat="1">
+    <row r="2" spans="1:31" s="18" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -738,19 +749,20 @@
       </c>
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
-      <c r="P2" s="17" t="s">
+      <c r="M2" s="19"/>
+      <c r="Q2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="V2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="X2" s="19"/>
       <c r="Y2" s="19"/>
-      <c r="Z2" s="17" t="s">
+      <c r="Z2" s="19"/>
+      <c r="AA2" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="5" customFormat="1">
+    <row r="3" spans="1:31" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -777,62 +789,63 @@
       <c r="L3" s="3">
         <v>43224</v>
       </c>
-      <c r="M3" s="3">
+      <c r="M3" s="3"/>
+      <c r="N3" s="3">
         <v>43229</v>
       </c>
-      <c r="N3" s="3">
+      <c r="O3" s="3">
         <v>43230</v>
       </c>
-      <c r="O3" s="3">
+      <c r="P3" s="3">
         <v>43231</v>
       </c>
-      <c r="P3" s="4">
+      <c r="Q3" s="4">
         <v>43234</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>43235</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>43236</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>43237</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>43238</v>
       </c>
-      <c r="U3" s="4">
+      <c r="V3" s="4">
         <v>43241</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>43242</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>43243</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>43244</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>43245</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>43248</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>43249</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>43250</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>43251</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:31">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -852,19 +865,16 @@
       <c r="L4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M4" t="s">
-        <v>3</v>
-      </c>
       <c r="N4" t="s">
         <v>3</v>
       </c>
       <c r="O4" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="P4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="R4" t="s">
@@ -876,25 +886,25 @@
       <c r="T4" t="s">
         <v>3</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="U4" t="s">
+        <v>3</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="W4" t="s">
         <v>3</v>
       </c>
-      <c r="X4" s="10" t="s">
+      <c r="X4" t="s">
         <v>3</v>
       </c>
       <c r="Y4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="Z4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AB4" t="s">
@@ -906,11 +916,14 @@
       <c r="AD4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:30">
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:30">
+      <c r="AE4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31">
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" spans="1:31">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -938,20 +951,23 @@
       <c r="L6" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="M6" s="10"/>
+      <c r="M6" s="20" t="s">
+        <v>74</v>
+      </c>
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="X6"/>
+      <c r="P6" s="10"/>
+      <c r="W6" s="10"/>
       <c r="Y6"/>
-      <c r="AA6" s="20"/>
+      <c r="Z6"/>
       <c r="AB6" s="20"/>
       <c r="AC6" s="20"/>
-      <c r="AD6" s="20" t="s">
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:31">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -982,18 +998,21 @@
       <c r="L7" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
-      <c r="V7" s="10"/>
-      <c r="X7"/>
+      <c r="P7" s="10"/>
+      <c r="W7" s="10"/>
       <c r="Y7"/>
-      <c r="AA7" s="20"/>
+      <c r="Z7"/>
       <c r="AB7" s="20"/>
       <c r="AC7" s="20"/>
       <c r="AD7" s="20"/>
-    </row>
-    <row r="8" spans="1:30">
+      <c r="AE7" s="20"/>
+    </row>
+    <row r="8" spans="1:31">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1024,15 +1043,21 @@
       <c r="K8" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="V8" s="10"/>
-      <c r="X8" s="7"/>
+      <c r="L8" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="W8" s="10"/>
       <c r="Y8" s="7"/>
-      <c r="AA8" s="20"/>
+      <c r="Z8" s="7"/>
       <c r="AB8" s="20"/>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
-    </row>
-    <row r="9" spans="1:30">
+      <c r="AE8" s="20"/>
+    </row>
+    <row r="9" spans="1:31">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1063,14 +1088,20 @@
       <c r="K9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="Q9" s="2"/>
-      <c r="V9" s="10"/>
-      <c r="X9" s="8"/>
+      <c r="L9" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="R9" s="2"/>
+      <c r="W9" s="10"/>
       <c r="Y9" s="8"/>
-      <c r="Z9" s="9"/>
-    </row>
-    <row r="10" spans="1:30">
+      <c r="Z9" s="8"/>
+      <c r="AA9" s="9"/>
+    </row>
+    <row r="10" spans="1:31">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1095,16 +1126,16 @@
       <c r="K10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="Q10" s="2"/>
-      <c r="V10" s="10"/>
-      <c r="X10" s="8"/>
+      <c r="R10" s="2"/>
+      <c r="W10" s="10"/>
       <c r="Y10" s="8"/>
-      <c r="AA10" s="20"/>
+      <c r="Z10" s="8"/>
       <c r="AB10" s="20"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="20"/>
-    </row>
-    <row r="11" spans="1:30">
+      <c r="AE10" s="20"/>
+    </row>
+    <row r="11" spans="1:31">
       <c r="D11" t="s">
         <v>42</v>
       </c>
@@ -1123,13 +1154,13 @@
       <c r="K11" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="Q11" s="2"/>
-      <c r="U11" s="9"/>
-      <c r="V11" s="10"/>
-      <c r="X11" s="8"/>
+      <c r="R11" s="2"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="10"/>
       <c r="Y11" s="8"/>
-    </row>
-    <row r="12" spans="1:30">
+      <c r="Z11" s="8"/>
+    </row>
+    <row r="12" spans="1:31">
       <c r="D12" t="s">
         <v>38</v>
       </c>
@@ -1139,16 +1170,16 @@
       <c r="K12" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="Q12" s="2"/>
-      <c r="V12" s="10"/>
-      <c r="X12" s="8"/>
+      <c r="R12" s="2"/>
+      <c r="W12" s="10"/>
       <c r="Y12" s="8"/>
-      <c r="AA12" s="7"/>
+      <c r="Z12" s="8"/>
       <c r="AB12" s="7"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
-    </row>
-    <row r="13" spans="1:30">
+      <c r="AE12" s="7"/>
+    </row>
+    <row r="13" spans="1:31">
       <c r="D13" t="s">
         <v>39</v>
       </c>
@@ -1161,17 +1192,17 @@
       <c r="K13" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="10"/>
-      <c r="Q13" s="2"/>
-      <c r="V13" s="10"/>
-      <c r="X13" s="8"/>
+      <c r="N13" s="10"/>
+      <c r="R13" s="2"/>
+      <c r="W13" s="10"/>
       <c r="Y13" s="8"/>
-      <c r="AA13" s="8"/>
+      <c r="Z13" s="8"/>
       <c r="AB13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8"/>
-    </row>
-    <row r="14" spans="1:30">
+      <c r="AE13" s="8"/>
+    </row>
+    <row r="14" spans="1:31">
       <c r="J14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1179,17 +1210,18 @@
         <v>34</v>
       </c>
       <c r="L14"/>
-      <c r="M14" s="10"/>
-      <c r="Q14" s="2"/>
-      <c r="V14" s="10"/>
-      <c r="X14" s="8"/>
+      <c r="M14"/>
+      <c r="N14" s="10"/>
+      <c r="R14" s="2"/>
+      <c r="W14" s="10"/>
       <c r="Y14" s="8"/>
-      <c r="AA14" s="8"/>
+      <c r="Z14" s="8"/>
       <c r="AB14" s="8"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
-    </row>
-    <row r="15" spans="1:30">
+      <c r="AE14" s="8"/>
+    </row>
+    <row r="15" spans="1:31">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1200,189 +1232,197 @@
       <c r="K15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="16" spans="1:30">
+      <c r="R15" s="2"/>
+    </row>
+    <row r="16" spans="1:31">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:20">
+    <row r="17" spans="4:21">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="I17" s="1"/>
-      <c r="N17" s="7"/>
       <c r="O17" s="7"/>
-    </row>
-    <row r="18" spans="4:20">
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="4:21">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="I18" s="1"/>
-      <c r="N18" s="8"/>
       <c r="O18" s="8"/>
-    </row>
-    <row r="19" spans="4:20">
+      <c r="P18" s="8"/>
+    </row>
+    <row r="19" spans="4:21">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="I19" s="1"/>
       <c r="L19"/>
-      <c r="N19" s="8"/>
+      <c r="M19"/>
       <c r="O19" s="8"/>
-    </row>
-    <row r="20" spans="4:20">
+      <c r="P19" s="8"/>
+    </row>
+    <row r="20" spans="4:21">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="I20" s="1"/>
       <c r="L20"/>
-      <c r="N20" s="8"/>
+      <c r="M20"/>
       <c r="O20" s="8"/>
-    </row>
-    <row r="21" spans="4:20">
+      <c r="P20" s="8"/>
+    </row>
+    <row r="21" spans="4:21">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
-      <c r="N21" s="8"/>
+      <c r="M21"/>
       <c r="O21" s="8"/>
-    </row>
-    <row r="22" spans="4:20">
+      <c r="P21" s="8"/>
+    </row>
+    <row r="22" spans="4:21">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
-      <c r="N22" s="8"/>
+      <c r="M22"/>
       <c r="O22" s="8"/>
-      <c r="R22" s="7"/>
+      <c r="P22" s="8"/>
       <c r="S22" s="7"/>
       <c r="T22" s="7"/>
-    </row>
-    <row r="23" spans="4:20">
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="4:21">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
-      <c r="N23" s="8"/>
+      <c r="M23"/>
       <c r="O23" s="8"/>
-      <c r="R23" s="8"/>
+      <c r="P23" s="8"/>
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
-    </row>
-    <row r="24" spans="4:20">
+      <c r="U23" s="8"/>
+    </row>
+    <row r="24" spans="4:21">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
-      <c r="N24" s="8"/>
+      <c r="M24"/>
       <c r="O24" s="8"/>
-      <c r="R24" s="8"/>
+      <c r="P24" s="8"/>
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
-    </row>
-    <row r="25" spans="4:20">
+      <c r="U24" s="8"/>
+    </row>
+    <row r="25" spans="4:21">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
-      <c r="R25" s="8"/>
       <c r="S25" s="8"/>
       <c r="T25" s="8"/>
-    </row>
-    <row r="26" spans="4:20">
+      <c r="U25" s="8"/>
+    </row>
+    <row r="26" spans="4:21">
       <c r="I26" s="1"/>
-      <c r="R26" s="8"/>
       <c r="S26" s="8"/>
       <c r="T26" s="8"/>
-    </row>
-    <row r="27" spans="4:20">
+      <c r="U26" s="8"/>
+    </row>
+    <row r="27" spans="4:21">
       <c r="I27" s="1"/>
-      <c r="R27" s="8"/>
       <c r="S27" s="8"/>
       <c r="T27" s="8"/>
-    </row>
-    <row r="28" spans="4:20">
+      <c r="U27" s="8"/>
+    </row>
+    <row r="28" spans="4:21">
       <c r="I28" s="1"/>
-      <c r="R28" s="8"/>
       <c r="S28" s="8"/>
       <c r="T28" s="8"/>
-    </row>
-    <row r="29" spans="4:20">
+      <c r="U28" s="8"/>
+    </row>
+    <row r="29" spans="4:21">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
-      <c r="R29" s="8"/>
       <c r="S29" s="8"/>
       <c r="T29" s="8"/>
-    </row>
-    <row r="30" spans="4:20">
+      <c r="U29" s="8"/>
+    </row>
+    <row r="30" spans="4:21">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
-      <c r="R30" s="8"/>
+      <c r="M30" s="14"/>
       <c r="S30" s="8"/>
       <c r="T30" s="8"/>
-    </row>
-    <row r="31" spans="4:20">
+      <c r="U30" s="8"/>
+    </row>
+    <row r="31" spans="4:21">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
-      <c r="R31" s="8"/>
       <c r="S31" s="8"/>
       <c r="T31" s="8"/>
-    </row>
-    <row r="32" spans="4:20">
+      <c r="U31" s="8"/>
+    </row>
+    <row r="32" spans="4:21">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
-      <c r="R32" s="8"/>
+      <c r="M32" s="14"/>
       <c r="S32" s="8"/>
       <c r="T32" s="8"/>
-    </row>
-    <row r="33" spans="8:20">
+      <c r="U32" s="8"/>
+    </row>
+    <row r="33" spans="8:21">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
-      <c r="R33" s="8"/>
       <c r="S33" s="8"/>
       <c r="T33" s="8"/>
-    </row>
-    <row r="34" spans="8:20">
+      <c r="U33" s="8"/>
+    </row>
+    <row r="34" spans="8:21">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
-      <c r="R34" s="8"/>
       <c r="S34" s="8"/>
       <c r="T34" s="8"/>
-    </row>
-    <row r="35" spans="8:20">
+      <c r="U34" s="8"/>
+    </row>
+    <row r="35" spans="8:21">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
-      <c r="R35" s="8"/>
       <c r="S35" s="8"/>
       <c r="T35" s="8"/>
-    </row>
-    <row r="36" spans="8:20">
+      <c r="U35" s="8"/>
+    </row>
+    <row r="36" spans="8:21">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:20">
+    <row r="37" spans="8:21">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:20">
+    <row r="38" spans="8:21">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:20">
+    <row r="41" spans="8:21">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:20">
+    <row r="42" spans="8:21">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:20">
+    <row r="43" spans="8:21">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:20">
+    <row r="44" spans="8:21">
       <c r="H44" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
opdateret IP og FP
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -263,6 +263,12 @@
   </si>
   <si>
     <t>15 min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementeret UC1 og UC2 </t>
+  </si>
+  <si>
+    <t>Opdateret SD for UC1 og UC2</t>
   </si>
 </sst>
 </file>
@@ -672,7 +678,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -687,7 +693,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1194,6 +1200,12 @@
       <c r="K12" s="20" t="s">
         <v>34</v>
       </c>
+      <c r="L12" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="M12" s="20" t="s">
+        <v>29</v>
+      </c>
       <c r="R12" s="2"/>
       <c r="W12" s="10"/>
       <c r="Y12" s="8"/>
@@ -1215,6 +1227,12 @@
       </c>
       <c r="K13" s="20" t="s">
         <v>44</v>
+      </c>
+      <c r="L13" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="M13" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="N13" s="10"/>
       <c r="R13" s="2"/>

</xml_diff>

<commit_message>
OC og supplerende krav føjet til rapport
iteration og faseplan opdateret. OC opdateret
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>Opdateret SD for UC1 og UC2</t>
+  </si>
+  <si>
+    <t>Rapport skrivning</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -687,13 +690,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AE44"/>
+  <dimension ref="A1:AF44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
+      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -712,22 +715,23 @@
     <col min="12" max="12" width="43" style="10" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.28515625" style="10" customWidth="1"/>
     <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="34.28515625" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="35" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="34.28515625" customWidth="1"/>
-    <col min="22" max="22" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.28515625" style="10" customWidth="1"/>
-    <col min="27" max="27" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="31" width="28.7109375" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="34.28515625" customWidth="1"/>
+    <col min="18" max="18" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="35" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="34.28515625" customWidth="1"/>
+    <col min="23" max="23" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.28515625" style="10" customWidth="1"/>
+    <col min="28" max="28" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="32" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:32" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -741,20 +745,20 @@
       <c r="K1" s="16"/>
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
-      <c r="O1" s="16"/>
       <c r="P1" s="16"/>
-      <c r="Q1" s="15"/>
-      <c r="V1" s="15" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="15"/>
+      <c r="W1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="X1" s="16"/>
       <c r="Y1" s="16"/>
       <c r="Z1" s="16"/>
-      <c r="AA1" s="15" t="s">
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="18" customFormat="1">
+    <row r="2" spans="1:32" s="18" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -768,19 +772,19 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="M2" s="19"/>
-      <c r="Q2" s="17" t="s">
+      <c r="R2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="W2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Y2" s="19"/>
       <c r="Z2" s="19"/>
-      <c r="AA2" s="17" t="s">
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:31" s="5" customFormat="1">
+    <row r="3" spans="1:32" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -809,61 +813,62 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="3">
-        <v>43229</v>
-      </c>
-      <c r="O3" s="3">
+        <v>43227</v>
+      </c>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3">
         <v>43230</v>
       </c>
-      <c r="P3" s="3">
+      <c r="Q3" s="3">
         <v>43231</v>
       </c>
-      <c r="Q3" s="4">
+      <c r="R3" s="4">
         <v>43234</v>
       </c>
-      <c r="R3" s="3">
+      <c r="S3" s="3">
         <v>43235</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>43236</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>43237</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>43238</v>
       </c>
-      <c r="V3" s="4">
+      <c r="W3" s="4">
         <v>43241</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>43242</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>43243</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>43244</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>43245</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>43248</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>43249</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>43250</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>43251</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:31">
+    <row r="4" spans="1:32">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -886,16 +891,13 @@
       <c r="N4" t="s">
         <v>3</v>
       </c>
-      <c r="O4" t="s">
-        <v>3</v>
-      </c>
       <c r="P4" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="Q4" t="s">
+        <v>3</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="S4" t="s">
@@ -907,25 +909,25 @@
       <c r="U4" t="s">
         <v>3</v>
       </c>
-      <c r="V4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W4" t="s">
+      <c r="V4" t="s">
+        <v>3</v>
+      </c>
+      <c r="W4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="X4" t="s">
         <v>3</v>
       </c>
-      <c r="Y4" s="10" t="s">
+      <c r="Y4" t="s">
         <v>3</v>
       </c>
       <c r="Z4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AB4" t="s">
+      <c r="AA4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AC4" t="s">
@@ -937,11 +939,15 @@
       <c r="AE4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="AF4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32">
       <c r="N5" s="10"/>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="O5" s="10"/>
+    </row>
+    <row r="6" spans="1:32">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -972,20 +978,23 @@
       <c r="M6" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
+      <c r="N6" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="O6" s="20"/>
       <c r="P6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="Y6"/>
+      <c r="Q6" s="10"/>
+      <c r="X6" s="10"/>
       <c r="Z6"/>
-      <c r="AB6" s="20"/>
+      <c r="AA6"/>
       <c r="AC6" s="20"/>
       <c r="AD6" s="20"/>
-      <c r="AE6" s="20" t="s">
+      <c r="AE6" s="20"/>
+      <c r="AF6" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:31">
+    <row r="7" spans="1:32">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1022,15 +1031,16 @@
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="10"/>
-      <c r="W7" s="10"/>
-      <c r="Y7"/>
+      <c r="Q7" s="10"/>
+      <c r="X7" s="10"/>
       <c r="Z7"/>
-      <c r="AB7" s="20"/>
+      <c r="AA7"/>
       <c r="AC7" s="20"/>
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="AF7" s="20"/>
+    </row>
+    <row r="8" spans="1:32">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1067,15 +1077,15 @@
       <c r="M8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="W8" s="10"/>
-      <c r="Y8" s="7"/>
+      <c r="X8" s="10"/>
       <c r="Z8" s="7"/>
-      <c r="AB8" s="20"/>
+      <c r="AA8" s="7"/>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
-    </row>
-    <row r="9" spans="1:31">
+      <c r="AF8" s="20"/>
+    </row>
+    <row r="9" spans="1:32">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1113,13 +1123,14 @@
         <v>29</v>
       </c>
       <c r="N9" s="10"/>
-      <c r="R9" s="2"/>
-      <c r="W9" s="10"/>
-      <c r="Y9" s="8"/>
+      <c r="O9" s="10"/>
+      <c r="S9" s="2"/>
+      <c r="X9" s="10"/>
       <c r="Z9" s="8"/>
-      <c r="AA9" s="9"/>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="9"/>
+    </row>
+    <row r="10" spans="1:32">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1150,16 +1161,16 @@
       <c r="M10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="R10" s="2"/>
-      <c r="W10" s="10"/>
-      <c r="Y10" s="8"/>
+      <c r="S10" s="2"/>
+      <c r="X10" s="10"/>
       <c r="Z10" s="8"/>
-      <c r="AB10" s="20"/>
+      <c r="AA10" s="8"/>
       <c r="AC10" s="20"/>
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
-    </row>
-    <row r="11" spans="1:31">
+      <c r="AF10" s="20"/>
+    </row>
+    <row r="11" spans="1:32">
       <c r="D11" t="s">
         <v>42</v>
       </c>
@@ -1184,13 +1195,13 @@
       <c r="M11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="R11" s="2"/>
-      <c r="V11" s="9"/>
-      <c r="W11" s="10"/>
-      <c r="Y11" s="8"/>
+      <c r="S11" s="2"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="10"/>
       <c r="Z11" s="8"/>
-    </row>
-    <row r="12" spans="1:31">
+      <c r="AA11" s="8"/>
+    </row>
+    <row r="12" spans="1:32">
       <c r="D12" t="s">
         <v>38</v>
       </c>
@@ -1206,16 +1217,16 @@
       <c r="M12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="R12" s="2"/>
-      <c r="W12" s="10"/>
-      <c r="Y12" s="8"/>
+      <c r="S12" s="2"/>
+      <c r="X12" s="10"/>
       <c r="Z12" s="8"/>
-      <c r="AB12" s="7"/>
+      <c r="AA12" s="8"/>
       <c r="AC12" s="7"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="AF12" s="7"/>
+    </row>
+    <row r="13" spans="1:32">
       <c r="D13" t="s">
         <v>39</v>
       </c>
@@ -1235,16 +1246,17 @@
         <v>34</v>
       </c>
       <c r="N13" s="10"/>
-      <c r="R13" s="2"/>
-      <c r="W13" s="10"/>
-      <c r="Y13" s="8"/>
+      <c r="O13" s="10"/>
+      <c r="S13" s="2"/>
+      <c r="X13" s="10"/>
       <c r="Z13" s="8"/>
-      <c r="AB13" s="8"/>
+      <c r="AA13" s="8"/>
       <c r="AC13" s="8"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="AF13" s="8"/>
+    </row>
+    <row r="14" spans="1:32">
       <c r="J14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1254,16 +1266,17 @@
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14" s="10"/>
-      <c r="R14" s="2"/>
-      <c r="W14" s="10"/>
-      <c r="Y14" s="8"/>
+      <c r="O14" s="10"/>
+      <c r="S14" s="2"/>
+      <c r="X14" s="10"/>
       <c r="Z14" s="8"/>
-      <c r="AB14" s="8"/>
+      <c r="AA14" s="8"/>
       <c r="AC14" s="8"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="AF14" s="8"/>
+    </row>
+    <row r="15" spans="1:32">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1274,34 +1287,34 @@
       <c r="K15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="R15" s="2"/>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" spans="1:32">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:21">
+    <row r="17" spans="4:22">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="I17" s="1"/>
-      <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-    </row>
-    <row r="18" spans="4:21">
+      <c r="Q17" s="7"/>
+    </row>
+    <row r="18" spans="4:22">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="I18" s="1"/>
-      <c r="O18" s="8"/>
       <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="4:21">
+      <c r="Q18" s="8"/>
+    </row>
+    <row r="19" spans="4:22">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1309,10 +1322,10 @@
       <c r="I19" s="1"/>
       <c r="L19"/>
       <c r="M19"/>
-      <c r="O19" s="8"/>
       <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="4:21">
+      <c r="Q19" s="8"/>
+    </row>
+    <row r="20" spans="4:22">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1320,151 +1333,151 @@
       <c r="I20" s="1"/>
       <c r="L20"/>
       <c r="M20"/>
-      <c r="O20" s="8"/>
       <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="4:21">
+      <c r="Q20" s="8"/>
+    </row>
+    <row r="21" spans="4:22">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
       <c r="M21"/>
-      <c r="O21" s="8"/>
       <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="4:21">
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="4:22">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
       <c r="M22"/>
-      <c r="O22" s="8"/>
       <c r="P22" s="8"/>
-      <c r="S22" s="7"/>
+      <c r="Q22" s="8"/>
       <c r="T22" s="7"/>
       <c r="U22" s="7"/>
-    </row>
-    <row r="23" spans="4:21">
+      <c r="V22" s="7"/>
+    </row>
+    <row r="23" spans="4:22">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
       <c r="M23"/>
-      <c r="O23" s="8"/>
       <c r="P23" s="8"/>
-      <c r="S23" s="8"/>
+      <c r="Q23" s="8"/>
       <c r="T23" s="8"/>
       <c r="U23" s="8"/>
-    </row>
-    <row r="24" spans="4:21">
+      <c r="V23" s="8"/>
+    </row>
+    <row r="24" spans="4:22">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
       <c r="M24"/>
-      <c r="O24" s="8"/>
       <c r="P24" s="8"/>
-      <c r="S24" s="8"/>
+      <c r="Q24" s="8"/>
       <c r="T24" s="8"/>
       <c r="U24" s="8"/>
-    </row>
-    <row r="25" spans="4:21">
+      <c r="V24" s="8"/>
+    </row>
+    <row r="25" spans="4:22">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
-      <c r="S25" s="8"/>
       <c r="T25" s="8"/>
       <c r="U25" s="8"/>
-    </row>
-    <row r="26" spans="4:21">
+      <c r="V25" s="8"/>
+    </row>
+    <row r="26" spans="4:22">
       <c r="I26" s="1"/>
-      <c r="S26" s="8"/>
       <c r="T26" s="8"/>
       <c r="U26" s="8"/>
-    </row>
-    <row r="27" spans="4:21">
+      <c r="V26" s="8"/>
+    </row>
+    <row r="27" spans="4:22">
       <c r="I27" s="1"/>
-      <c r="S27" s="8"/>
       <c r="T27" s="8"/>
       <c r="U27" s="8"/>
-    </row>
-    <row r="28" spans="4:21">
+      <c r="V27" s="8"/>
+    </row>
+    <row r="28" spans="4:22">
       <c r="I28" s="1"/>
-      <c r="S28" s="8"/>
       <c r="T28" s="8"/>
       <c r="U28" s="8"/>
-    </row>
-    <row r="29" spans="4:21">
+      <c r="V28" s="8"/>
+    </row>
+    <row r="29" spans="4:22">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
-      <c r="S29" s="8"/>
       <c r="T29" s="8"/>
       <c r="U29" s="8"/>
-    </row>
-    <row r="30" spans="4:21">
+      <c r="V29" s="8"/>
+    </row>
+    <row r="30" spans="4:22">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
-      <c r="S30" s="8"/>
       <c r="T30" s="8"/>
       <c r="U30" s="8"/>
-    </row>
-    <row r="31" spans="4:21">
+      <c r="V30" s="8"/>
+    </row>
+    <row r="31" spans="4:22">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
-      <c r="S31" s="8"/>
       <c r="T31" s="8"/>
       <c r="U31" s="8"/>
-    </row>
-    <row r="32" spans="4:21">
+      <c r="V31" s="8"/>
+    </row>
+    <row r="32" spans="4:22">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
-      <c r="S32" s="8"/>
       <c r="T32" s="8"/>
       <c r="U32" s="8"/>
-    </row>
-    <row r="33" spans="8:21">
+      <c r="V32" s="8"/>
+    </row>
+    <row r="33" spans="8:22">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
-      <c r="S33" s="8"/>
       <c r="T33" s="8"/>
       <c r="U33" s="8"/>
-    </row>
-    <row r="34" spans="8:21">
+      <c r="V33" s="8"/>
+    </row>
+    <row r="34" spans="8:22">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
-      <c r="S34" s="8"/>
       <c r="T34" s="8"/>
       <c r="U34" s="8"/>
-    </row>
-    <row r="35" spans="8:21">
+      <c r="V34" s="8"/>
+    </row>
+    <row r="35" spans="8:22">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
-      <c r="S35" s="8"/>
       <c r="T35" s="8"/>
       <c r="U35" s="8"/>
-    </row>
-    <row r="36" spans="8:21">
+      <c r="V35" s="8"/>
+    </row>
+    <row r="36" spans="8:22">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:21">
+    <row r="37" spans="8:22">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:21">
+    <row r="38" spans="8:22">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:21">
+    <row r="41" spans="8:22">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:21">
+    <row r="42" spans="8:22">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:21">
+    <row r="43" spans="8:22">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:21">
+    <row r="44" spans="8:22">
       <c r="H44" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rettelser i SD opdateret IP/FP
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="87">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -272,6 +272,15 @@
   </si>
   <si>
     <t>Rapport skrivning</t>
+  </si>
+  <si>
+    <t>5 timer</t>
+  </si>
+  <si>
+    <t>review af gruppe 2</t>
+  </si>
+  <si>
+    <t>Klargøring af fremlæggelse</t>
   </si>
 </sst>
 </file>
@@ -681,7 +690,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -690,13 +699,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AF44"/>
+  <dimension ref="A1:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="O1" sqref="O1"/>
+      <selection pane="bottomRight" activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -717,21 +726,22 @@
     <col min="14" max="14" width="35.28515625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="14" customWidth="1"/>
     <col min="16" max="16" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.28515625" customWidth="1"/>
-    <col min="18" max="18" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="35" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="34.28515625" customWidth="1"/>
-    <col min="23" max="23" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.28515625" style="10" customWidth="1"/>
-    <col min="28" max="28" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="32" width="28.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.28515625" customWidth="1"/>
+    <col min="19" max="19" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="35" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="34.28515625" customWidth="1"/>
+    <col min="24" max="24" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.28515625" style="10" customWidth="1"/>
+    <col min="29" max="29" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="33" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:33" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -747,18 +757,19 @@
       <c r="M1" s="16"/>
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
-      <c r="R1" s="15"/>
-      <c r="W1" s="15" t="s">
+      <c r="R1" s="16"/>
+      <c r="S1" s="15"/>
+      <c r="X1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Y1" s="16"/>
       <c r="Z1" s="16"/>
       <c r="AA1" s="16"/>
-      <c r="AB1" s="15" t="s">
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:32" s="18" customFormat="1">
+    <row r="2" spans="1:33" s="18" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>18</v>
       </c>
@@ -772,19 +783,19 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="M2" s="19"/>
-      <c r="R2" s="17" t="s">
+      <c r="S2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="17" t="s">
+      <c r="X2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="Z2" s="19"/>
       <c r="AA2" s="19"/>
-      <c r="AB2" s="17" t="s">
+      <c r="AB2" s="19"/>
+      <c r="AC2" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="5" customFormat="1">
+    <row r="3" spans="1:33" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>20</v>
       </c>
@@ -819,56 +830,57 @@
       <c r="P3" s="3">
         <v>43230</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3">
         <v>43231</v>
       </c>
-      <c r="R3" s="4">
+      <c r="S3" s="4">
         <v>43234</v>
       </c>
-      <c r="S3" s="3">
+      <c r="T3" s="3">
         <v>43235</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>43236</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>43237</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>43238</v>
       </c>
-      <c r="W3" s="4">
+      <c r="X3" s="4">
         <v>43241</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Y3" s="3">
         <v>43242</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>43243</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>43244</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>43245</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>43248</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>43249</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>43250</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>43251</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:32">
+    <row r="4" spans="1:33">
       <c r="A4" s="6" t="s">
         <v>19</v>
       </c>
@@ -894,13 +906,10 @@
       <c r="P4" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" t="s">
-        <v>3</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="S4" t="s">
+      <c r="R4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="T4" t="s">
@@ -912,25 +921,25 @@
       <c r="V4" t="s">
         <v>3</v>
       </c>
-      <c r="W4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="W4" t="s">
+        <v>3</v>
+      </c>
+      <c r="X4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Y4" t="s">
         <v>3</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" t="s">
         <v>3</v>
       </c>
       <c r="AA4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AB4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AC4" t="s">
+      <c r="AB4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AD4" t="s">
@@ -942,12 +951,15 @@
       <c r="AF4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:32">
+      <c r="AG4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33">
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:32">
+    <row r="6" spans="1:33">
       <c r="B6" s="1" t="s">
         <v>26</v>
       </c>
@@ -981,20 +993,27 @@
       <c r="N6" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="O6" s="20"/>
-      <c r="P6" s="10"/>
-      <c r="Q6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Z6"/>
+      <c r="O6" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="P6" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q6" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="R6" s="10"/>
+      <c r="Y6" s="10"/>
       <c r="AA6"/>
-      <c r="AC6" s="20"/>
+      <c r="AB6"/>
       <c r="AD6" s="20"/>
       <c r="AE6" s="20"/>
-      <c r="AF6" s="20" t="s">
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="20" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:32">
+    <row r="7" spans="1:33">
       <c r="B7" s="1" t="s">
         <v>22</v>
       </c>
@@ -1030,17 +1049,20 @@
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
+      <c r="P7" s="20" t="s">
+        <v>86</v>
+      </c>
       <c r="Q7" s="10"/>
-      <c r="X7" s="10"/>
-      <c r="Z7"/>
+      <c r="R7" s="10"/>
+      <c r="Y7" s="10"/>
       <c r="AA7"/>
-      <c r="AC7" s="20"/>
+      <c r="AB7"/>
       <c r="AD7" s="20"/>
       <c r="AE7" s="20"/>
       <c r="AF7" s="20"/>
-    </row>
-    <row r="8" spans="1:32">
+      <c r="AG7" s="20"/>
+    </row>
+    <row r="8" spans="1:33">
       <c r="B8" s="1" t="s">
         <v>23</v>
       </c>
@@ -1077,15 +1099,15 @@
       <c r="M8" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="X8" s="10"/>
-      <c r="Z8" s="7"/>
+      <c r="Y8" s="10"/>
       <c r="AA8" s="7"/>
-      <c r="AC8" s="20"/>
+      <c r="AB8" s="7"/>
       <c r="AD8" s="20"/>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
-    </row>
-    <row r="9" spans="1:32">
+      <c r="AG8" s="20"/>
+    </row>
+    <row r="9" spans="1:33">
       <c r="B9" s="1" t="s">
         <v>24</v>
       </c>
@@ -1124,13 +1146,13 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="S9" s="2"/>
-      <c r="X9" s="10"/>
-      <c r="Z9" s="8"/>
+      <c r="T9" s="2"/>
+      <c r="Y9" s="10"/>
       <c r="AA9" s="8"/>
-      <c r="AB9" s="9"/>
-    </row>
-    <row r="10" spans="1:32">
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="9"/>
+    </row>
+    <row r="10" spans="1:33">
       <c r="B10" s="1" t="s">
         <v>27</v>
       </c>
@@ -1161,16 +1183,16 @@
       <c r="M10" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="S10" s="2"/>
-      <c r="X10" s="10"/>
-      <c r="Z10" s="8"/>
+      <c r="T10" s="2"/>
+      <c r="Y10" s="10"/>
       <c r="AA10" s="8"/>
-      <c r="AC10" s="20"/>
+      <c r="AB10" s="8"/>
       <c r="AD10" s="20"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
-    </row>
-    <row r="11" spans="1:32">
+      <c r="AG10" s="20"/>
+    </row>
+    <row r="11" spans="1:33">
       <c r="D11" t="s">
         <v>42</v>
       </c>
@@ -1195,13 +1217,13 @@
       <c r="M11" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="S11" s="2"/>
-      <c r="W11" s="9"/>
-      <c r="X11" s="10"/>
-      <c r="Z11" s="8"/>
+      <c r="T11" s="2"/>
+      <c r="X11" s="9"/>
+      <c r="Y11" s="10"/>
       <c r="AA11" s="8"/>
-    </row>
-    <row r="12" spans="1:32">
+      <c r="AB11" s="8"/>
+    </row>
+    <row r="12" spans="1:33">
       <c r="D12" t="s">
         <v>38</v>
       </c>
@@ -1217,16 +1239,16 @@
       <c r="M12" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="S12" s="2"/>
-      <c r="X12" s="10"/>
-      <c r="Z12" s="8"/>
+      <c r="T12" s="2"/>
+      <c r="Y12" s="10"/>
       <c r="AA12" s="8"/>
-      <c r="AC12" s="7"/>
+      <c r="AB12" s="8"/>
       <c r="AD12" s="7"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
-    </row>
-    <row r="13" spans="1:32">
+      <c r="AG12" s="7"/>
+    </row>
+    <row r="13" spans="1:33">
       <c r="D13" t="s">
         <v>39</v>
       </c>
@@ -1247,16 +1269,16 @@
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="S13" s="2"/>
-      <c r="X13" s="10"/>
-      <c r="Z13" s="8"/>
+      <c r="T13" s="2"/>
+      <c r="Y13" s="10"/>
       <c r="AA13" s="8"/>
-      <c r="AC13" s="8"/>
+      <c r="AB13" s="8"/>
       <c r="AD13" s="8"/>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
-    </row>
-    <row r="14" spans="1:32">
+      <c r="AG13" s="8"/>
+    </row>
+    <row r="14" spans="1:33">
       <c r="J14" s="1" t="s">
         <v>70</v>
       </c>
@@ -1267,16 +1289,16 @@
       <c r="M14"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="S14" s="2"/>
-      <c r="X14" s="10"/>
-      <c r="Z14" s="8"/>
+      <c r="T14" s="2"/>
+      <c r="Y14" s="10"/>
       <c r="AA14" s="8"/>
-      <c r="AC14" s="8"/>
+      <c r="AB14" s="8"/>
       <c r="AD14" s="8"/>
       <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
-    </row>
-    <row r="15" spans="1:32">
+      <c r="AG14" s="8"/>
+    </row>
+    <row r="15" spans="1:33">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1287,16 +1309,16 @@
       <c r="K15" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="S15" s="2"/>
-    </row>
-    <row r="16" spans="1:32">
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" spans="1:33">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:22">
+    <row r="17" spans="4:23">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1304,8 +1326,9 @@
       <c r="I17" s="1"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
-    </row>
-    <row r="18" spans="4:22">
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" spans="4:23">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1313,8 +1336,9 @@
       <c r="I18" s="1"/>
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
-    </row>
-    <row r="19" spans="4:22">
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="4:23">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1324,8 +1348,9 @@
       <c r="M19"/>
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
-    </row>
-    <row r="20" spans="4:22">
+      <c r="R19" s="8"/>
+    </row>
+    <row r="20" spans="4:23">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1335,149 +1360,154 @@
       <c r="M20"/>
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
-    </row>
-    <row r="21" spans="4:22">
+      <c r="R20" s="8"/>
+    </row>
+    <row r="21" spans="4:23">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
       <c r="M21"/>
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
-    </row>
-    <row r="22" spans="4:22">
+      <c r="R21" s="8"/>
+    </row>
+    <row r="22" spans="4:23">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
       <c r="M22"/>
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
-      <c r="T22" s="7"/>
+      <c r="R22" s="8"/>
       <c r="U22" s="7"/>
       <c r="V22" s="7"/>
-    </row>
-    <row r="23" spans="4:22">
+      <c r="W22" s="7"/>
+    </row>
+    <row r="23" spans="4:23">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
       <c r="M23"/>
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
-      <c r="T23" s="8"/>
+      <c r="R23" s="8"/>
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
-    </row>
-    <row r="24" spans="4:22">
+      <c r="W23" s="8"/>
+    </row>
+    <row r="24" spans="4:23">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
       <c r="M24"/>
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
-      <c r="T24" s="8"/>
+      <c r="R24" s="8"/>
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
-    </row>
-    <row r="25" spans="4:22">
+      <c r="W24" s="8"/>
+    </row>
+    <row r="25" spans="4:23">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
-      <c r="T25" s="8"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
-    </row>
-    <row r="26" spans="4:22">
+      <c r="W25" s="8"/>
+    </row>
+    <row r="26" spans="4:23">
       <c r="I26" s="1"/>
-      <c r="T26" s="8"/>
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
-    </row>
-    <row r="27" spans="4:22">
+      <c r="W26" s="8"/>
+    </row>
+    <row r="27" spans="4:23">
       <c r="I27" s="1"/>
-      <c r="T27" s="8"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
-    </row>
-    <row r="28" spans="4:22">
+      <c r="W27" s="8"/>
+    </row>
+    <row r="28" spans="4:23">
       <c r="I28" s="1"/>
-      <c r="T28" s="8"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
-    </row>
-    <row r="29" spans="4:22">
+      <c r="W28" s="8"/>
+    </row>
+    <row r="29" spans="4:23">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
-      <c r="T29" s="8"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
-    </row>
-    <row r="30" spans="4:22">
+      <c r="W29" s="8"/>
+    </row>
+    <row r="30" spans="4:23">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
-      <c r="T30" s="8"/>
       <c r="U30" s="8"/>
       <c r="V30" s="8"/>
-    </row>
-    <row r="31" spans="4:22">
+      <c r="W30" s="8"/>
+    </row>
+    <row r="31" spans="4:23">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
-      <c r="T31" s="8"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
-    </row>
-    <row r="32" spans="4:22">
+      <c r="W31" s="8"/>
+    </row>
+    <row r="32" spans="4:23">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
-      <c r="T32" s="8"/>
       <c r="U32" s="8"/>
       <c r="V32" s="8"/>
-    </row>
-    <row r="33" spans="8:22">
+      <c r="W32" s="8"/>
+    </row>
+    <row r="33" spans="8:23">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
-      <c r="T33" s="8"/>
       <c r="U33" s="8"/>
       <c r="V33" s="8"/>
-    </row>
-    <row r="34" spans="8:22">
+      <c r="W33" s="8"/>
+    </row>
+    <row r="34" spans="8:23">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
-      <c r="T34" s="8"/>
       <c r="U34" s="8"/>
       <c r="V34" s="8"/>
-    </row>
-    <row r="35" spans="8:22">
+      <c r="W34" s="8"/>
+    </row>
+    <row r="35" spans="8:23">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
-      <c r="T35" s="8"/>
       <c r="U35" s="8"/>
       <c r="V35" s="8"/>
-    </row>
-    <row r="36" spans="8:22">
+      <c r="W35" s="8"/>
+    </row>
+    <row r="36" spans="8:23">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:22">
+    <row r="37" spans="8:23">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:22">
+    <row r="38" spans="8:23">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:22">
+    <row r="41" spans="8:23">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:22">
+    <row r="42" spans="8:23">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:22">
+    <row r="43" spans="8:23">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:22">
+    <row r="44" spans="8:23">
       <c r="H44" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
faseplan + fremlæggelse af milepæl a
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -1,18 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
   <workbookPr codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloms\OneDrive\Dokumenter\GitHub\FFT\modeller, dokumenter\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="68" documentId="11_F2E9B523360FAD3B3FB31BC29CA991CEDBF64511" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{A02F3242-B97C-4610-9EC6-29811CE934CF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
     <sheet name="Milepæle" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="118">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -58,15 +64,6 @@
     <t>Iterationsplan for E1 er klar</t>
   </si>
   <si>
-    <t>I0</t>
-  </si>
-  <si>
-    <t>E1</t>
-  </si>
-  <si>
-    <t>E2</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -202,9 +199,6 @@
     <t>Sekvens diagram for UC1 og UC2</t>
   </si>
   <si>
-    <t>Opdatere klasse diagram</t>
-  </si>
-  <si>
     <t>Implementere UC1 og UC2.</t>
   </si>
   <si>
@@ -290,13 +284,109 @@
   </si>
   <si>
     <t>skriver om MUST</t>
+  </si>
+  <si>
+    <t>UC1-3 er fuldt beskrevet</t>
+  </si>
+  <si>
+    <t>Arkitekturen er stabil og beskrevet</t>
+  </si>
+  <si>
+    <t>Alle UC's er identificeret</t>
+  </si>
+  <si>
+    <t>Eksekverbart produkt er udarbejdet (use cases implementeret)</t>
+  </si>
+  <si>
+    <t>Systemet er fuldt implementeret (alle UC's)</t>
+  </si>
+  <si>
+    <t>Systemet består alle systemtests</t>
+  </si>
+  <si>
+    <t>Interessenter er parat til systemets udrulning</t>
+  </si>
+  <si>
+    <t>Systemet er leveret og i drift</t>
+  </si>
+  <si>
+    <t>Systemet består accepttest</t>
+  </si>
+  <si>
+    <t>Brugerne er tilfredse</t>
+  </si>
+  <si>
+    <t>Påbegynd fase- og iterationsplan</t>
+  </si>
+  <si>
+    <t>Påbegynd visionsdokument</t>
+  </si>
+  <si>
+    <t>Opsæt udviklingsmiljø</t>
+  </si>
+  <si>
+    <t>Påbegynd risikoanalyse</t>
+  </si>
+  <si>
+    <t>Påbegynd domænemodel</t>
+  </si>
+  <si>
+    <t>Udarbejd mock-ups</t>
+  </si>
+  <si>
+    <t>Formel beskrivelse af UC1-2</t>
+  </si>
+  <si>
+    <t>Identificer use cases</t>
+  </si>
+  <si>
+    <t>Review i samarbejde med gruppe 2</t>
+  </si>
+  <si>
+    <t>Systemsekvensdiagram for UC1-3</t>
+  </si>
+  <si>
+    <t>Operationskontrakt for UC1 og UC2</t>
+  </si>
+  <si>
+    <t>Opdatere klassediagram</t>
+  </si>
+  <si>
+    <t>Påbegynd datamodel</t>
+  </si>
+  <si>
+    <t>Påbegynd dataordbog</t>
+  </si>
+  <si>
+    <t>Opdater dataorbog</t>
+  </si>
+  <si>
+    <t>Operationskontrakt til UC3</t>
+  </si>
+  <si>
+    <t>Aktivitetsdiagram for UC3</t>
+  </si>
+  <si>
+    <t>Implementation af UC3</t>
+  </si>
+  <si>
+    <t>Uformel beskrivelse af yderligere use cases</t>
+  </si>
+  <si>
+    <t>I0 30/4 - 3/5</t>
+  </si>
+  <si>
+    <t>E1 3/5 - 14/5</t>
+  </si>
+  <si>
+    <t>E2 14/5 - 21/5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +423,29 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -387,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,6 +540,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,25 +817,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Ark1"/>
   <dimension ref="A1:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="N4" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="P3" sqref="P3"/>
+      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -750,9 +868,9 @@
     <col min="30" max="33" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:33" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="15" t="s">
         <v>4</v>
@@ -778,12 +896,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="18" customFormat="1">
+    <row r="2" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="19"/>
       <c r="J2" s="17" t="s">
@@ -801,12 +919,12 @@
       <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
       <c r="AC2" s="17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:33" s="5" customFormat="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" s="4">
         <v>43220</v>
@@ -889,9 +1007,9 @@
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -964,52 +1082,52 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>29</v>
-      </c>
       <c r="D6" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="O6" s="20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="P6" s="20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="Q6" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="R6" s="10"/>
       <c r="Y6" s="10"/>
@@ -1019,47 +1137,47 @@
       <c r="AE6" s="20"/>
       <c r="AF6" s="20"/>
       <c r="AG6" s="20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:33">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="K7" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N7" s="10"/>
       <c r="O7" s="10"/>
       <c r="P7" s="20" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="10"/>
       <c r="R7" s="10"/>
@@ -1071,45 +1189,45 @@
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F8" s="20" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="Y8" s="10"/>
       <c r="AA8" s="7"/>
@@ -1119,42 +1237,42 @@
       <c r="AF8" s="20"/>
       <c r="AG8" s="20"/>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F9" s="20" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
@@ -1164,36 +1282,36 @@
       <c r="AB9" s="8"/>
       <c r="AC9" s="9"/>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="K10" s="20" t="s">
-        <v>44</v>
-      </c>
       <c r="L10" s="20" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="T10" s="2"/>
       <c r="Y10" s="10"/>
@@ -1204,30 +1322,30 @@
       <c r="AF10" s="20"/>
       <c r="AG10" s="20"/>
     </row>
-    <row r="11" spans="1:33">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E11" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11" s="20" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="K11" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="T11" s="2"/>
       <c r="X11" s="9"/>
@@ -1235,21 +1353,21 @@
       <c r="AA11" s="8"/>
       <c r="AB11" s="8"/>
     </row>
-    <row r="12" spans="1:33">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="T12" s="2"/>
       <c r="Y12" s="10"/>
@@ -1260,24 +1378,24 @@
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
     </row>
-    <row r="13" spans="1:33">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
@@ -1290,12 +1408,12 @@
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
     </row>
-    <row r="14" spans="1:33">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="J14" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L14"/>
       <c r="M14"/>
@@ -1310,27 +1428,27 @@
       <c r="AF14" s="8"/>
       <c r="AG14" s="8"/>
     </row>
-    <row r="15" spans="1:33">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="I15" s="9"/>
       <c r="J15" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="T15" s="2"/>
     </row>
-    <row r="16" spans="1:33">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:23">
+    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1340,7 +1458,7 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="4:23">
+    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1350,7 +1468,7 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="4:23">
+    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1362,7 +1480,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="4:23">
+    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1374,7 +1492,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="4:23">
+    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
@@ -1383,7 +1501,7 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="4:23">
+    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
@@ -1395,7 +1513,7 @@
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
     </row>
-    <row r="23" spans="4:23">
+    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
@@ -1407,7 +1525,7 @@
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
     </row>
-    <row r="24" spans="4:23">
+    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
@@ -1419,39 +1537,39 @@
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
     </row>
-    <row r="25" spans="4:23">
+    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
       <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
     </row>
-    <row r="26" spans="4:23">
+    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I26" s="1"/>
       <c r="U26" s="8"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
     </row>
-    <row r="27" spans="4:23">
+    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I27" s="1"/>
       <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
     </row>
-    <row r="28" spans="4:23">
+    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I28" s="1"/>
       <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
     </row>
-    <row r="29" spans="4:23">
+    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
       <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
     </row>
-    <row r="30" spans="4:23">
+    <row r="30" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
@@ -1460,14 +1578,14 @@
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
     </row>
-    <row r="31" spans="4:23">
+    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
       <c r="U31" s="8"/>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
     </row>
-    <row r="32" spans="4:23">
+    <row r="32" spans="4:23" x14ac:dyDescent="0.25">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
@@ -1477,7 +1595,7 @@
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
     </row>
-    <row r="33" spans="8:23">
+    <row r="33" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
@@ -1485,7 +1603,7 @@
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
     </row>
-    <row r="34" spans="8:23">
+    <row r="34" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
@@ -1493,7 +1611,7 @@
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
     </row>
-    <row r="35" spans="8:23">
+    <row r="35" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
@@ -1501,25 +1619,25 @@
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
     </row>
-    <row r="36" spans="8:23">
+    <row r="36" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:23">
+    <row r="37" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:23">
+    <row r="38" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:23">
+    <row r="41" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:23">
+    <row r="42" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:23">
+    <row r="43" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:23">
+    <row r="44" spans="8:23" x14ac:dyDescent="0.25">
       <c r="H44" s="8"/>
     </row>
   </sheetData>
@@ -1529,29 +1647,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Ark2"/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
+      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>4</v>
@@ -1559,101 +1678,228 @@
       <c r="C1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="21" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1">
+    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E2" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="F2" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" t="s">
         <v>55</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="C4" t="s">
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C11" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="C6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="C7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="C9" t="s">
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>110</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="C10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
-      <c r="A15" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="B16" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2">
-      <c r="B17" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2">
-      <c r="B18" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2">
-      <c r="B19" s="8" t="s">
+      <c r="E19" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="8" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
opdatering af IP/FP og Log
</commit_message>
<xml_diff>
--- a/modeller, dokumenter/Iteration og faseplan.xlsx
+++ b/modeller, dokumenter/Iteration og faseplan.xlsx
@@ -1,24 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloms\OneDrive\Dokumenter\GitHub\FFT\modeller, dokumenter\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="11_F2E9B523360FAD3B3FB31BC29CA991CEDBF64511" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{A02F3242-B97C-4610-9EC6-29811CE934CF}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Overordnet projektplan" sheetId="1" r:id="rId1"/>
     <sheet name="Milepæle" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="121">
   <si>
     <t>Klargøring af projektplan</t>
   </si>
@@ -380,13 +374,22 @@
   </si>
   <si>
     <t>E2 14/5 - 21/5</t>
+  </si>
+  <si>
+    <t>påbegynde GUI</t>
+  </si>
+  <si>
+    <t>1,5timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fremlæggelser </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -817,25 +820,25 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark1"/>
-  <dimension ref="A1:AG44"/>
+  <dimension ref="A1:AH44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="O4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -855,20 +858,21 @@
     <col min="16" max="16" width="34.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="34.28515625" customWidth="1"/>
-    <col min="19" max="19" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="35" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="34.28515625" customWidth="1"/>
-    <col min="24" max="24" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="35.28515625" style="10" customWidth="1"/>
-    <col min="29" max="29" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="33" width="28.7109375" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="35" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="34.28515625" customWidth="1"/>
+    <col min="25" max="25" width="35.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="34.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="35.28515625" style="10" customWidth="1"/>
+    <col min="30" max="30" width="28.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="34" width="28.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -885,18 +889,19 @@
       <c r="P1" s="16"/>
       <c r="Q1" s="16"/>
       <c r="R1" s="16"/>
-      <c r="S1" s="15"/>
-      <c r="X1" s="15" t="s">
+      <c r="S1" s="16"/>
+      <c r="T1" s="15"/>
+      <c r="Y1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="Z1" s="16"/>
       <c r="AA1" s="16"/>
       <c r="AB1" s="16"/>
-      <c r="AC1" s="15" t="s">
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:33" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" s="18" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
@@ -910,19 +915,19 @@
       <c r="K2" s="19"/>
       <c r="L2" s="19"/>
       <c r="M2" s="19"/>
-      <c r="S2" s="17" t="s">
+      <c r="T2" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="17" t="s">
+      <c r="Y2" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="AA2" s="19"/>
       <c r="AB2" s="19"/>
-      <c r="AC2" s="17" t="s">
+      <c r="AC2" s="19"/>
+      <c r="AD2" s="17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:33" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" s="5" customFormat="1">
       <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
@@ -959,55 +964,56 @@
       </c>
       <c r="Q3" s="3"/>
       <c r="R3" s="3">
-        <v>43231</v>
-      </c>
-      <c r="S3" s="4">
+        <v>43229</v>
+      </c>
+      <c r="S3" s="3"/>
+      <c r="T3" s="4">
         <v>43234</v>
       </c>
-      <c r="T3" s="3">
+      <c r="U3" s="3">
         <v>43235</v>
       </c>
-      <c r="U3" s="3">
+      <c r="V3" s="3">
         <v>43236</v>
       </c>
-      <c r="V3" s="3">
+      <c r="W3" s="3">
         <v>43237</v>
       </c>
-      <c r="W3" s="3">
+      <c r="X3" s="3">
         <v>43238</v>
       </c>
-      <c r="X3" s="4">
+      <c r="Y3" s="4">
         <v>43241</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Z3" s="3">
         <v>43242</v>
       </c>
-      <c r="Z3" s="3">
+      <c r="AA3" s="3">
         <v>43243</v>
       </c>
-      <c r="AA3" s="3">
+      <c r="AB3" s="3">
         <v>43244</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AC3" s="3">
         <v>43245</v>
       </c>
-      <c r="AC3" s="3">
+      <c r="AD3" s="3">
         <v>43248</v>
       </c>
-      <c r="AD3" s="3">
+      <c r="AE3" s="3">
         <v>43249</v>
       </c>
-      <c r="AE3" s="3">
+      <c r="AF3" s="3">
         <v>43250</v>
       </c>
-      <c r="AF3" s="3">
+      <c r="AG3" s="3">
         <v>43251</v>
       </c>
-      <c r="AG3" s="3">
+      <c r="AH3" s="3">
         <v>43252</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34">
       <c r="A4" s="6" t="s">
         <v>16</v>
       </c>
@@ -1036,10 +1042,7 @@
       <c r="R4" t="s">
         <v>3</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="T4" t="s">
+      <c r="T4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="U4" t="s">
@@ -1051,25 +1054,25 @@
       <c r="W4" t="s">
         <v>3</v>
       </c>
-      <c r="X4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y4" t="s">
+      <c r="X4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Z4" t="s">
         <v>3</v>
       </c>
-      <c r="AA4" s="10" t="s">
+      <c r="AA4" t="s">
         <v>3</v>
       </c>
       <c r="AB4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="AD4" t="s">
+      <c r="AC4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="AE4" t="s">
@@ -1081,12 +1084,15 @@
       <c r="AG4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34">
       <c r="N5" s="10"/>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34">
       <c r="B6" s="1" t="s">
         <v>23</v>
       </c>
@@ -1129,18 +1135,23 @@
       <c r="Q6" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="R6" s="10"/>
-      <c r="Y6" s="10"/>
-      <c r="AA6"/>
+      <c r="R6" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="S6" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z6" s="10"/>
       <c r="AB6"/>
-      <c r="AD6" s="20"/>
+      <c r="AC6"/>
       <c r="AE6" s="20"/>
       <c r="AF6" s="20"/>
-      <c r="AG6" s="20" t="s">
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34">
       <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
@@ -1179,17 +1190,20 @@
       <c r="P7" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="Q7" s="10"/>
+      <c r="Q7" s="20" t="s">
+        <v>119</v>
+      </c>
       <c r="R7" s="10"/>
-      <c r="Y7" s="10"/>
-      <c r="AA7"/>
+      <c r="S7" s="10"/>
+      <c r="Z7" s="10"/>
       <c r="AB7"/>
-      <c r="AD7" s="20"/>
+      <c r="AC7"/>
       <c r="AE7" s="20"/>
       <c r="AF7" s="20"/>
       <c r="AG7" s="20"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH7" s="20"/>
+    </row>
+    <row r="8" spans="1:34">
       <c r="B8" s="1" t="s">
         <v>20</v>
       </c>
@@ -1229,15 +1243,18 @@
       <c r="P8" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="Y8" s="10"/>
-      <c r="AA8" s="7"/>
+      <c r="Q8" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z8" s="10"/>
       <c r="AB8" s="7"/>
-      <c r="AD8" s="20"/>
+      <c r="AC8" s="7"/>
       <c r="AE8" s="20"/>
       <c r="AF8" s="20"/>
       <c r="AG8" s="20"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH8" s="20"/>
+    </row>
+    <row r="9" spans="1:34">
       <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
@@ -1276,13 +1293,19 @@
       </c>
       <c r="N9" s="10"/>
       <c r="O9" s="10"/>
-      <c r="T9" s="2"/>
-      <c r="Y9" s="10"/>
-      <c r="AA9" s="8"/>
+      <c r="P9" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>46</v>
+      </c>
+      <c r="U9" s="2"/>
+      <c r="Z9" s="10"/>
       <c r="AB9" s="8"/>
-      <c r="AC9" s="9"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AC9" s="8"/>
+      <c r="AD9" s="9"/>
+    </row>
+    <row r="10" spans="1:34">
       <c r="B10" s="1" t="s">
         <v>24</v>
       </c>
@@ -1313,16 +1336,16 @@
       <c r="M10" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="T10" s="2"/>
-      <c r="Y10" s="10"/>
-      <c r="AA10" s="8"/>
+      <c r="U10" s="2"/>
+      <c r="Z10" s="10"/>
       <c r="AB10" s="8"/>
-      <c r="AD10" s="20"/>
+      <c r="AC10" s="8"/>
       <c r="AE10" s="20"/>
       <c r="AF10" s="20"/>
       <c r="AG10" s="20"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH10" s="20"/>
+    </row>
+    <row r="11" spans="1:34">
       <c r="D11" t="s">
         <v>39</v>
       </c>
@@ -1347,13 +1370,13 @@
       <c r="M11" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="T11" s="2"/>
-      <c r="X11" s="9"/>
-      <c r="Y11" s="10"/>
-      <c r="AA11" s="8"/>
+      <c r="U11" s="2"/>
+      <c r="Y11" s="9"/>
+      <c r="Z11" s="10"/>
       <c r="AB11" s="8"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AC11" s="8"/>
+    </row>
+    <row r="12" spans="1:34">
       <c r="D12" t="s">
         <v>35</v>
       </c>
@@ -1369,16 +1392,16 @@
       <c r="M12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="2"/>
-      <c r="Y12" s="10"/>
-      <c r="AA12" s="8"/>
+      <c r="U12" s="2"/>
+      <c r="Z12" s="10"/>
       <c r="AB12" s="8"/>
-      <c r="AD12" s="7"/>
+      <c r="AC12" s="8"/>
       <c r="AE12" s="7"/>
       <c r="AF12" s="7"/>
       <c r="AG12" s="7"/>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH12" s="7"/>
+    </row>
+    <row r="13" spans="1:34">
       <c r="D13" t="s">
         <v>36</v>
       </c>
@@ -1399,16 +1422,16 @@
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10"/>
-      <c r="T13" s="2"/>
-      <c r="Y13" s="10"/>
-      <c r="AA13" s="8"/>
+      <c r="U13" s="2"/>
+      <c r="Z13" s="10"/>
       <c r="AB13" s="8"/>
-      <c r="AD13" s="8"/>
+      <c r="AC13" s="8"/>
       <c r="AE13" s="8"/>
       <c r="AF13" s="8"/>
       <c r="AG13" s="8"/>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH13" s="8"/>
+    </row>
+    <row r="14" spans="1:34">
       <c r="J14" s="1" t="s">
         <v>66</v>
       </c>
@@ -1419,16 +1442,16 @@
       <c r="M14"/>
       <c r="N14" s="10"/>
       <c r="O14" s="10"/>
-      <c r="T14" s="2"/>
-      <c r="Y14" s="10"/>
-      <c r="AA14" s="8"/>
+      <c r="U14" s="2"/>
+      <c r="Z14" s="10"/>
       <c r="AB14" s="8"/>
-      <c r="AD14" s="8"/>
+      <c r="AC14" s="8"/>
       <c r="AE14" s="8"/>
       <c r="AF14" s="8"/>
       <c r="AG14" s="8"/>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH14" s="8"/>
+    </row>
+    <row r="15" spans="1:34">
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
@@ -1439,16 +1462,16 @@
       <c r="K15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="T15" s="2"/>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="1:34">
       <c r="D16" s="7"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="I16" s="1"/>
     </row>
-    <row r="17" spans="4:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:24">
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1457,8 +1480,9 @@
       <c r="P17" s="7"/>
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
-    </row>
-    <row r="18" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="S17" s="7"/>
+    </row>
+    <row r="18" spans="4:24">
       <c r="D18" s="8"/>
       <c r="E18" s="8"/>
       <c r="F18" s="8"/>
@@ -1467,8 +1491,9 @@
       <c r="P18" s="8"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
-    </row>
-    <row r="19" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="4:24">
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
       <c r="F19" s="8"/>
@@ -1479,8 +1504,9 @@
       <c r="P19" s="8"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
-    </row>
-    <row r="20" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="4:24">
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
@@ -1491,8 +1517,9 @@
       <c r="P20" s="8"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
-    </row>
-    <row r="21" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="4:24">
       <c r="D21" s="8"/>
       <c r="I21" s="1"/>
       <c r="L21"/>
@@ -1500,8 +1527,9 @@
       <c r="P21" s="8"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
-    </row>
-    <row r="22" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="4:24">
       <c r="H22" s="8"/>
       <c r="I22" s="1"/>
       <c r="L22"/>
@@ -1509,11 +1537,12 @@
       <c r="P22" s="8"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
-      <c r="U22" s="7"/>
+      <c r="S22" s="8"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
-    </row>
-    <row r="23" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X22" s="7"/>
+    </row>
+    <row r="23" spans="4:24">
       <c r="H23" s="8"/>
       <c r="I23" s="1"/>
       <c r="L23"/>
@@ -1521,11 +1550,12 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
-      <c r="U23" s="8"/>
+      <c r="S23" s="8"/>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
-    </row>
-    <row r="24" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X23" s="8"/>
+    </row>
+    <row r="24" spans="4:24">
       <c r="H24" s="8"/>
       <c r="I24" s="1"/>
       <c r="L24"/>
@@ -1533,111 +1563,112 @@
       <c r="P24" s="8"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
-      <c r="U24" s="8"/>
+      <c r="S24" s="8"/>
       <c r="V24" s="8"/>
       <c r="W24" s="8"/>
-    </row>
-    <row r="25" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X24" s="8"/>
+    </row>
+    <row r="25" spans="4:24">
       <c r="H25" s="8"/>
       <c r="I25" s="1"/>
-      <c r="U25" s="8"/>
       <c r="V25" s="8"/>
       <c r="W25" s="8"/>
-    </row>
-    <row r="26" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X25" s="8"/>
+    </row>
+    <row r="26" spans="4:24">
       <c r="I26" s="1"/>
-      <c r="U26" s="8"/>
       <c r="V26" s="8"/>
       <c r="W26" s="8"/>
-    </row>
-    <row r="27" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X26" s="8"/>
+    </row>
+    <row r="27" spans="4:24">
       <c r="I27" s="1"/>
-      <c r="U27" s="8"/>
       <c r="V27" s="8"/>
       <c r="W27" s="8"/>
-    </row>
-    <row r="28" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X27" s="8"/>
+    </row>
+    <row r="28" spans="4:24">
       <c r="I28" s="1"/>
-      <c r="U28" s="8"/>
       <c r="V28" s="8"/>
       <c r="W28" s="8"/>
-    </row>
-    <row r="29" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X28" s="8"/>
+    </row>
+    <row r="29" spans="4:24">
       <c r="I29" s="1"/>
       <c r="K29" s="14"/>
-      <c r="U29" s="8"/>
       <c r="V29" s="8"/>
       <c r="W29" s="8"/>
-    </row>
-    <row r="30" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X29" s="8"/>
+    </row>
+    <row r="30" spans="4:24">
       <c r="I30" s="2"/>
       <c r="K30" s="14"/>
       <c r="L30" s="14"/>
       <c r="M30" s="14"/>
-      <c r="U30" s="8"/>
       <c r="V30" s="8"/>
       <c r="W30" s="8"/>
-    </row>
-    <row r="31" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X30" s="8"/>
+    </row>
+    <row r="31" spans="4:24">
       <c r="I31" s="2"/>
       <c r="K31" s="14"/>
-      <c r="U31" s="8"/>
       <c r="V31" s="8"/>
       <c r="W31" s="8"/>
-    </row>
-    <row r="32" spans="4:23" x14ac:dyDescent="0.25">
+      <c r="X31" s="8"/>
+    </row>
+    <row r="32" spans="4:24">
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="K32" s="14"/>
       <c r="L32" s="14"/>
       <c r="M32" s="14"/>
-      <c r="U32" s="8"/>
       <c r="V32" s="8"/>
       <c r="W32" s="8"/>
-    </row>
-    <row r="33" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="X32" s="8"/>
+    </row>
+    <row r="33" spans="8:24">
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="K33" s="14"/>
-      <c r="U33" s="8"/>
       <c r="V33" s="8"/>
       <c r="W33" s="8"/>
-    </row>
-    <row r="34" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="8:24">
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="K34" s="14"/>
-      <c r="U34" s="8"/>
       <c r="V34" s="8"/>
       <c r="W34" s="8"/>
-    </row>
-    <row r="35" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="X34" s="8"/>
+    </row>
+    <row r="35" spans="8:24">
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="K35" s="14"/>
-      <c r="U35" s="8"/>
       <c r="V35" s="8"/>
       <c r="W35" s="8"/>
-    </row>
-    <row r="36" spans="8:23" x14ac:dyDescent="0.25">
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="8:24">
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:24">
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:24">
       <c r="H38" s="2"/>
     </row>
-    <row r="41" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="41" spans="8:24">
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="42" spans="8:24">
       <c r="H42" s="8"/>
     </row>
-    <row r="43" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="43" spans="8:24">
       <c r="H43" s="8"/>
     </row>
-    <row r="44" spans="8:23" x14ac:dyDescent="0.25">
+    <row r="44" spans="8:24">
       <c r="H44" s="8"/>
     </row>
   </sheetData>
@@ -1647,18 +1678,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Ark2"/>
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
@@ -1668,7 +1699,7 @@
     <col min="6" max="6" width="27.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="11" customFormat="1" ht="18.75">
       <c r="A1" s="11" t="s">
         <v>14</v>
       </c>
@@ -1685,7 +1716,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" s="12" customFormat="1">
       <c r="A2" s="13" t="s">
         <v>15</v>
       </c>
@@ -1705,7 +1736,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" s="6" t="s">
         <v>52</v>
       </c>
@@ -1721,7 +1752,7 @@
       <c r="E3" s="23"/>
       <c r="F3" s="23"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="B4" t="s">
         <v>96</v>
       </c>
@@ -1734,7 +1765,7 @@
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="B5" t="s">
         <v>97</v>
       </c>
@@ -1747,7 +1778,7 @@
       <c r="E5" s="23"/>
       <c r="F5" s="23"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="B6" t="s">
         <v>103</v>
       </c>
@@ -1760,7 +1791,7 @@
       <c r="E6" s="23"/>
       <c r="F6" s="23"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="B7" t="s">
         <v>99</v>
       </c>
@@ -1773,7 +1804,7 @@
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="B8" t="s">
         <v>100</v>
       </c>
@@ -1783,7 +1814,7 @@
       <c r="E8" s="23"/>
       <c r="F8" s="23"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="B9" t="s">
         <v>102</v>
       </c>
@@ -1793,7 +1824,7 @@
       <c r="E9" s="23"/>
       <c r="F9" s="23"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="B10" t="s">
         <v>101</v>
       </c>
@@ -1803,7 +1834,7 @@
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="B11" t="s">
         <v>104</v>
       </c>
@@ -1813,7 +1844,7 @@
       <c r="E11" s="23"/>
       <c r="F11" s="23"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6">
       <c r="B12" t="s">
         <v>109</v>
       </c>
@@ -1823,29 +1854,29 @@
       <c r="E12" s="23"/>
       <c r="F12" s="23"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="C13" t="s">
         <v>84</v>
       </c>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="C14" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="23"/>
       <c r="F14" s="23"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6">
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6">
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6">
       <c r="A17" s="6" t="s">
         <v>1</v>
       </c>
@@ -1862,7 +1893,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6">
       <c r="B18" s="8" t="s">
         <v>28</v>
       </c>
@@ -1876,7 +1907,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6">
       <c r="B19" s="8" t="s">
         <v>27</v>
       </c>
@@ -1890,7 +1921,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6">
       <c r="B20" s="8" t="s">
         <v>29</v>
       </c>
@@ -1898,7 +1929,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6">
       <c r="B21" s="8" t="s">
         <v>11</v>
       </c>

</xml_diff>